<commit_message>
aanpassingen teamkalender adhv taakstructuur
</commit_message>
<xml_diff>
--- a/TeamKalender2302 (3).xlsx
+++ b/TeamKalender2302 (3).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2465ff4d818e327/Documenten/Camille/fase1 sem2/p^0o2/InTeDienen2302/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2465ff4d818e327/groep-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{116DC1BB-4E5F-428F-8C78-0669CAF09A2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{116DC1BB-4E5F-428F-8C78-0669CAF09A2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F8AF8AB7-D91A-4427-9DCB-1A49088BCF65}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F2D6B72F-93C9-4FC9-97EC-F6469066DD8B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>week</t>
   </si>
@@ -102,9 +102,6 @@
     <t>demonstratie</t>
   </si>
   <si>
-    <t>eindpresentatie en verslag</t>
-  </si>
-  <si>
     <t>inleiding en brainstorm</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>route beschikbaar</t>
   </si>
   <si>
-    <t>tussentijds verslag</t>
-  </si>
-  <si>
     <t xml:space="preserve">slides presentatie </t>
   </si>
   <si>
@@ -171,10 +165,19 @@
     <t>planning [1.5-1.9]</t>
   </si>
   <si>
-    <t>tests wagen [4]</t>
-  </si>
-  <si>
     <t>verbetering docs [1.5-1.9]</t>
+  </si>
+  <si>
+    <t>tussentijds verslag [5.1]</t>
+  </si>
+  <si>
+    <t>eindpresentatie en verslag [5.2, 5.3]</t>
+  </si>
+  <si>
+    <t>tests wagen [4.2]</t>
+  </si>
+  <si>
+    <t>test zonder parcour [4.1]</t>
   </si>
 </sst>
 </file>
@@ -460,6 +463,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -469,10 +476,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="4" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Controlecel" xfId="3" builtinId="23"/>
@@ -795,7 +798,7 @@
   <dimension ref="B2:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -813,31 +816,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
+      <c r="B2" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
     </row>
     <row r="3" spans="2:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="2:12" ht="26.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -869,7 +872,7 @@
         <v>16</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -884,13 +887,13 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="7"/>
       <c r="L6" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
@@ -900,22 +903,22 @@
       <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="19" t="s">
-        <v>42</v>
+      <c r="D7" s="16" t="s">
+        <v>40</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="7"/>
       <c r="L7" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
@@ -925,25 +928,27 @@
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>42</v>
+      <c r="D8" s="16" t="s">
+        <v>40</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="19" t="s">
-        <v>41</v>
+      <c r="G8" s="16" t="s">
+        <v>39</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="9"/>
+      <c r="L8" s="9" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="12">
@@ -960,9 +965,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="7"/>
-      <c r="L9" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="L9" s="9"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="12">
@@ -1010,13 +1013,13 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="11" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="7"/>
       <c r="L12" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1035,21 +1038,21 @@
       <c r="J13" s="3"/>
       <c r="K13" s="7"/>
       <c r="L13" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="2:12" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
       <c r="K14" s="7"/>
       <c r="L14" s="9"/>
     </row>
@@ -1064,7 +1067,9 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="7"/>
@@ -1082,13 +1087,13 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="7"/>
       <c r="L16" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
@@ -1109,7 +1114,7 @@
       <c r="J17" s="3"/>
       <c r="K17" s="7"/>
       <c r="L17" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
@@ -1128,7 +1133,7 @@
       <c r="J18" s="3"/>
       <c r="K18" s="7"/>
       <c r="L18" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1143,45 +1148,45 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="5" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="7"/>
       <c r="L19" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B21" s="18" t="s">
-        <v>44</v>
+      <c r="B21" s="15" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B22" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
+      <c r="B22" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B25" s="18"/>
+      <c r="B25" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>